<commit_message>
attempt to split and handle pagerank as slices - incredibly slow
</commit_message>
<xml_diff>
--- a/numbers.xlsx
+++ b/numbers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>for</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>ALL these are in seconds</t>
+  </si>
+  <si>
+    <t>map - split</t>
+  </si>
+  <si>
+    <t>mapPar-split</t>
+  </si>
+  <si>
+    <t>split</t>
   </si>
 </sst>
 </file>
@@ -411,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +438,14 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -452,8 +467,26 @@
       <c r="I2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>4.7005929442189801E-2</v>
       </c>
@@ -475,8 +508,26 @@
       <c r="I3">
         <v>13.9212853079708</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3">
+        <v>0.31519290773303998</v>
+      </c>
+      <c r="L3">
+        <v>1.0316822960826699</v>
+      </c>
+      <c r="M3">
+        <v>7.3807045950577493E-2</v>
+      </c>
+      <c r="O3">
+        <v>0.30653552513797999</v>
+      </c>
+      <c r="P3">
+        <v>1.01931440411138</v>
+      </c>
+      <c r="Q3">
+        <v>5.9332231192476902E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>7.5449859680265893E-2</v>
       </c>
@@ -498,8 +549,26 @@
       <c r="I4">
         <v>12.946096710497001</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="K4">
+        <v>0.40530568339822298</v>
+      </c>
+      <c r="L4">
+        <v>1.10064360867004</v>
+      </c>
+      <c r="M4">
+        <v>6.48689293637362E-2</v>
+      </c>
+      <c r="O4">
+        <v>0.41344602392760998</v>
+      </c>
+      <c r="P4">
+        <v>1.14696613516254</v>
+      </c>
+      <c r="Q4">
+        <v>6.6403041379433897E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>4.1315631022901901E-2</v>
       </c>
@@ -521,8 +590,26 @@
       <c r="I5">
         <v>13.0394138236442</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="K5">
+        <v>0.41530198753994702</v>
+      </c>
+      <c r="L5">
+        <v>1.22933320478174</v>
+      </c>
+      <c r="M5">
+        <v>0.13133624653926801</v>
+      </c>
+      <c r="O5">
+        <v>0.54558571791810595</v>
+      </c>
+      <c r="P5">
+        <v>1.2081992285014</v>
+      </c>
+      <c r="Q5">
+        <v>5.9687638535608503E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>3.3253272157899499E-2</v>
       </c>
@@ -544,8 +631,26 @@
       <c r="I6">
         <v>12.7394150524462</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6">
+        <v>0.40404048997061198</v>
+      </c>
+      <c r="L6">
+        <v>1.12248556393976</v>
+      </c>
+      <c r="M6">
+        <v>6.5359977541281297E-2</v>
+      </c>
+      <c r="O6">
+        <v>0.36761501822880399</v>
+      </c>
+      <c r="P6">
+        <v>1.0544482159213</v>
+      </c>
+      <c r="Q6">
+        <v>5.8096812582176402E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>3.7103203297726303E-2</v>
       </c>
@@ -567,8 +672,26 @@
       <c r="I7">
         <v>12.525866281768</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K7">
+        <v>0.38736233873155501</v>
+      </c>
+      <c r="L7">
+        <v>1.22485658462995</v>
+      </c>
+      <c r="M7">
+        <v>5.7353859997862799E-2</v>
+      </c>
+      <c r="O7">
+        <v>0.41728839320907302</v>
+      </c>
+      <c r="P7">
+        <v>1.3216601870992799</v>
+      </c>
+      <c r="Q7">
+        <v>6.6089696873454104E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <f>AVERAGE(A3:A7)</f>
         <v>4.6825579120196678E-2</v>
@@ -580,6 +703,14 @@
       <c r="G9">
         <f>AVERAGE(G3:G7)</f>
         <v>6.7094856896557892E-2</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGE(K3:K7)</f>
+        <v>0.38544068147467542</v>
+      </c>
+      <c r="O9">
+        <f>AVERAGE(O3:O7)</f>
+        <v>0.41009413568431458</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +723,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>